<commit_message>
Revert "Merge branch 'main' of https://github.com/fu-syoji-t/SD3D_2023_Scrum1"
This reverts commit 9bc7e03e0fa480d840583de198b0efedc6149126, reversing
changes made to 601193047c60ae4d9fd7d0bcc7f8b190ef1fad73.
</commit_message>
<xml_diff>
--- a/02プロダクトバックログ/Scrum1_プロダクトバックログ.xlsx
+++ b/02プロダクトバックログ/Scrum1_プロダクトバックログ.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48004438-F8D6-4F6A-8E8F-45C6DB653ED4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577ADC24-E1AC-4AB1-84F6-1CD4B5DE8AE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>チーム名</t>
     <rPh sb="3" eb="4">
@@ -285,13 +285,6 @@
     <t>第2スプリントで実装（7割）</t>
     <rPh sb="12" eb="13">
       <t>ワリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>第3スプリント</t>
-    <rPh sb="0" eb="1">
-      <t>ダイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -707,7 +700,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -814,9 +807,7 @@
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="1">
@@ -831,9 +822,7 @@
       <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="39.950000000000003" customHeight="1">
       <c r="A8" s="1">

</xml_diff>